<commit_message>
Add notes from class
</commit_message>
<xml_diff>
--- a/optimisation/docs/lectures/New Bedford Steel Example.xlsx
+++ b/optimisation/docs/lectures/New Bedford Steel Example.xlsx
@@ -4,60 +4,60 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="105" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sensitivity Report 1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Responses" sheetId="3" r:id="rId3"/>
+    <sheet name="Responses" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet1!$B$17:$I$17</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet1!$B$24</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet1!$B$25</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Sheet1!$B$26:$B$27</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Sheet1!$B$28</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Sheet1!$B$29:$B$36</definedName>
-    <definedName name="solver_lhs6" localSheetId="1" hidden="1">Sheet1!$B$37:$B$44</definedName>
-    <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">6</definedName>
-    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">Sheet1!$C$24</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Sheet1!$C$25</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Sheet1!$C$26:$C$27</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">Sheet1!$C$28</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">Sheet1!$C$29:$C$36</definedName>
-    <definedName name="solver_rhs6" localSheetId="1" hidden="1">Sheet1!$C$37:$C$44</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Sheet1!$B$17:$I$17</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">Sheet1!$B$24</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">Sheet1!$B$25</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">Sheet1!$B$26:$B$27</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">Sheet1!$B$28</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">Sheet1!$B$29:$B$36</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">Sheet1!$B$37:$B$44</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">6</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">Sheet1!$C$24</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">Sheet1!$C$25</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">Sheet1!$C$26:$C$27</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">Sheet1!$C$28</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">Sheet1!$C$29:$C$36</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">Sheet1!$C$37:$C$44</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.05</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="139">
   <si>
     <t>Ashley</t>
   </si>
@@ -434,9 +434,6 @@
     <t>How much does an extra ton of coking coal cost NBS?</t>
   </si>
   <si>
-    <t>At the current rate, 61500</t>
-  </si>
-  <si>
     <t>Should NBS consider expanding their trucking capacity? If so, how much should they be willing to spend?</t>
   </si>
   <si>
@@ -471,6 +468,24 @@
   </si>
   <si>
     <t>No. Currently spending less through union mines, and cost per mt is less than non-union</t>
+  </si>
+  <si>
+    <t>At the current rate, 61500/mt therefore 61.50</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Add note about range- this is only valid for up to 5 extra mega tons</t>
+  </si>
+  <si>
+    <t>Again, note that this is only valid within a certain range</t>
+  </si>
+  <si>
+    <t>Y - ish</t>
+  </si>
+  <si>
+    <t>It doesn't cost NBS anything; the shadow price is 0</t>
   </si>
 </sst>
 </file>
@@ -479,7 +494,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -827,15 +842,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -852,7 +858,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="32">
     <cellStyle name="Comma" xfId="31" builtinId="3"/>
@@ -1217,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1234,17 +1249,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1254,334 +1269,334 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="37" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickBot="1">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="45" t="s">
+      <c r="J8" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="K8" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="K8" s="45" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="39">
         <v>55.000000000000099</v>
       </c>
-      <c r="E9" s="42">
-        <v>0</v>
-      </c>
-      <c r="F9" s="38">
+      <c r="E9" s="39">
+        <v>0</v>
+      </c>
+      <c r="F9" s="35">
         <v>49500</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="35">
         <v>499.99999999998437</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="35">
         <v>1000.0000000000382</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9" s="34">
         <v>1</v>
       </c>
-      <c r="J9" s="46">
+      <c r="J9" s="43">
         <f>I9*F9*D9</f>
         <v>2722500.0000000051</v>
       </c>
-      <c r="K9" s="46">
+      <c r="K9" s="43">
         <f>IF(I9=1,0,D9*F9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="39">
         <v>600</v>
       </c>
-      <c r="E10" s="42">
-        <v>0</v>
-      </c>
-      <c r="F10" s="38">
+      <c r="E10" s="39">
+        <v>0</v>
+      </c>
+      <c r="F10" s="35">
         <v>49999.999999999993</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="35">
         <v>1499.9999999999918</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="35">
         <v>1E+30</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="34">
         <v>1</v>
       </c>
-      <c r="J10" s="46">
+      <c r="J10" s="43">
         <f t="shared" ref="J10:J15" si="0">I10*F10*D10</f>
         <v>29999999.999999996</v>
       </c>
-      <c r="K10" s="46">
+      <c r="K10" s="43">
         <f t="shared" ref="K10:K16" si="1">IF(I10=1,0,D10*F10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="42">
-        <v>0</v>
-      </c>
-      <c r="E11" s="42">
-        <v>0</v>
-      </c>
-      <c r="F11" s="38">
+      <c r="D11" s="39">
+        <v>0</v>
+      </c>
+      <c r="E11" s="39">
+        <v>0</v>
+      </c>
+      <c r="F11" s="35">
         <v>61000.000000000007</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="35">
         <v>2499.9999999999773</v>
       </c>
-      <c r="I11" s="37">
-        <v>0</v>
-      </c>
-      <c r="J11" s="46">
+      <c r="I11" s="34">
+        <v>0</v>
+      </c>
+      <c r="J11" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K11" s="46">
+      <c r="K11" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="39">
         <v>19.999999999999464</v>
       </c>
-      <c r="E12" s="42">
-        <v>0</v>
-      </c>
-      <c r="F12" s="38">
+      <c r="E12" s="39">
+        <v>0</v>
+      </c>
+      <c r="F12" s="35">
         <v>63499.999999999993</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="35">
         <v>125.00000000000455</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="35">
         <v>49.999999999998352</v>
       </c>
-      <c r="I12" s="37">
+      <c r="I12" s="34">
         <v>1</v>
       </c>
-      <c r="J12" s="46">
+      <c r="J12" s="43">
         <f t="shared" si="0"/>
         <v>1269999.9999999658</v>
       </c>
-      <c r="K12" s="46">
+      <c r="K12" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="39">
         <v>100.00000000000065</v>
       </c>
-      <c r="E13" s="42">
-        <v>0</v>
-      </c>
-      <c r="F13" s="38">
+      <c r="E13" s="39">
+        <v>0</v>
+      </c>
+      <c r="F13" s="35">
         <v>66500</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="35">
         <v>49.999999999998352</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="35">
         <v>125.00000000000455</v>
       </c>
-      <c r="I13" s="37">
-        <v>0</v>
-      </c>
-      <c r="J13" s="46">
+      <c r="I13" s="34">
+        <v>0</v>
+      </c>
+      <c r="J13" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="46">
+      <c r="K13" s="43">
         <f t="shared" si="1"/>
         <v>6650000.0000000438</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="39">
         <v>8.7707618945387341E-14</v>
       </c>
-      <c r="E14" s="42">
-        <v>0</v>
-      </c>
-      <c r="F14" s="38">
+      <c r="E14" s="39">
+        <v>0</v>
+      </c>
+      <c r="F14" s="35">
         <v>71000</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H14" s="38">
+      <c r="H14" s="35">
         <v>1500.0000000000168</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I14" s="34">
         <v>1</v>
       </c>
-      <c r="J14" s="46">
+      <c r="J14" s="43">
         <f t="shared" si="0"/>
         <v>6.2272409451225014E-9</v>
       </c>
-      <c r="K14" s="46">
+      <c r="K14" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="39">
         <v>450</v>
       </c>
-      <c r="E15" s="42">
-        <v>0</v>
-      </c>
-      <c r="F15" s="38">
+      <c r="E15" s="39">
+        <v>0</v>
+      </c>
+      <c r="F15" s="35">
         <v>72500</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="35">
         <v>1000.0000000000382</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="35">
         <v>1.6888498602639389E+20</v>
       </c>
-      <c r="I15" s="37">
-        <v>0</v>
-      </c>
-      <c r="J15" s="46">
+      <c r="I15" s="34">
+        <v>0</v>
+      </c>
+      <c r="J15" s="43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="46">
+      <c r="K15" s="43">
         <f t="shared" si="1"/>
         <v>32625000</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="40">
         <v>2.2204460492502539E-15</v>
       </c>
-      <c r="E16" s="43">
-        <v>0</v>
-      </c>
-      <c r="F16" s="39">
+      <c r="E16" s="40">
+        <v>0</v>
+      </c>
+      <c r="F16" s="36">
         <v>80000</v>
       </c>
-      <c r="G16" s="39">
+      <c r="G16" s="36">
         <v>2.7021597764223001E+19</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="36">
         <v>499.99999999998374</v>
       </c>
-      <c r="I16" s="37">
-        <v>0</v>
-      </c>
-      <c r="J16" s="46">
+      <c r="I16" s="34">
+        <v>0</v>
+      </c>
+      <c r="J16" s="43">
         <f t="shared" ref="J16" si="2">I16*F16*D16</f>
         <v>0</v>
       </c>
-      <c r="K16" s="46">
+      <c r="K16" s="43">
         <f t="shared" si="1"/>
         <v>1.7763568394002032E-10</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="J17" s="46">
+      <c r="J17" s="43">
         <f>SUM(J9:J16)</f>
         <v>33992499.99999997</v>
       </c>
-      <c r="K17" s="46">
+      <c r="K17" s="43">
         <f>SUM(K9:K16)</f>
         <v>39275000.000000045</v>
       </c>
@@ -1591,550 +1606,554 @@
         <v>21</v>
       </c>
       <c r="I18" t="s">
-        <v>131</v>
-      </c>
-      <c r="J18" s="46">
+        <v>130</v>
+      </c>
+      <c r="J18" s="43">
         <f>SUMIF($I$9:$I$16,1,$D$9:$D$16)</f>
         <v>674.99999999999966</v>
       </c>
-      <c r="K18" s="46">
+      <c r="K18" s="43">
         <f>SUMIF($I$9:$I$16,0,$D$9:$D$16)</f>
         <v>550.00000000000068</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40" t="s">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="40" t="s">
+      <c r="G19" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="H19" s="40" t="s">
+      <c r="H19" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="J19" s="46">
+      <c r="I19" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="J19" s="43">
         <f>J17/J18</f>
         <v>50359.259259259241</v>
       </c>
-      <c r="K19" s="46">
+      <c r="K19" s="43">
         <f>K17/K18</f>
         <v>71409.090909090897</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16.5" thickBot="1">
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="41" t="s">
+      <c r="F20" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="38" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="39">
         <v>1225.0000000000005</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="39">
         <v>61500.000000000036</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="35">
         <v>1225</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="35">
         <v>4.999999999999857</v>
       </c>
-      <c r="H21" s="38">
+      <c r="H21" s="35">
         <v>25.000000000000117</v>
       </c>
+      <c r="I21">
+        <f>E21/1000</f>
+        <v>61.500000000000036</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="42">
+      <c r="D22" s="39">
         <v>124.99999999999898</v>
       </c>
-      <c r="E22" s="42">
-        <v>0</v>
-      </c>
-      <c r="F22" s="38">
-        <v>0</v>
-      </c>
-      <c r="G22" s="38">
+      <c r="E22" s="39">
+        <v>0</v>
+      </c>
+      <c r="F22" s="35">
+        <v>0</v>
+      </c>
+      <c r="G22" s="35">
         <v>124.99999999999883</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="35">
         <v>1E+30</v>
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="42">
+      <c r="D23" s="39">
         <v>505.00000000000011</v>
       </c>
-      <c r="E23" s="42">
-        <v>0</v>
-      </c>
-      <c r="F23" s="38">
+      <c r="E23" s="39">
+        <v>0</v>
+      </c>
+      <c r="F23" s="35">
         <v>650</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="35">
         <v>145.00000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D24" s="39">
         <v>720.00000000000023</v>
       </c>
-      <c r="E24" s="42">
+      <c r="E24" s="39">
         <v>-1000.0000000000471</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="35">
         <v>720</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="35">
         <v>20.000000000000096</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="35">
         <v>3.3333333333332389</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="44">
+      <c r="D25" s="41">
         <v>1.0791367799356519E-14</v>
       </c>
-      <c r="E25" s="44">
+      <c r="E25" s="41">
         <v>300000.00000000052</v>
       </c>
-      <c r="F25" s="38">
-        <v>0</v>
-      </c>
-      <c r="G25" s="38">
+      <c r="F25" s="35">
+        <v>0</v>
+      </c>
+      <c r="G25" s="35">
         <v>0.19999999999999446</v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="35">
         <v>1.0000000000000058</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="39">
         <v>55.000000000000099</v>
       </c>
-      <c r="E26" s="42">
-        <v>0</v>
-      </c>
-      <c r="F26" s="38">
+      <c r="E26" s="39">
+        <v>0</v>
+      </c>
+      <c r="F26" s="35">
         <v>300</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H26" s="38">
+      <c r="H26" s="35">
         <v>244.99999999999994</v>
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="39">
         <v>600</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="39">
         <v>-1499.9999999999918</v>
       </c>
-      <c r="F27" s="38">
+      <c r="F27" s="35">
         <v>600</v>
       </c>
-      <c r="G27" s="38">
+      <c r="G27" s="35">
         <v>3.9999999999998872</v>
       </c>
-      <c r="H27" s="38">
+      <c r="H27" s="35">
         <v>25.000000000000117</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="42">
-        <v>0</v>
-      </c>
-      <c r="E28" s="42">
-        <v>0</v>
-      </c>
-      <c r="F28" s="38">
+      <c r="D28" s="39">
+        <v>0</v>
+      </c>
+      <c r="E28" s="39">
+        <v>0</v>
+      </c>
+      <c r="F28" s="35">
         <v>510</v>
       </c>
-      <c r="G28" s="38">
+      <c r="G28" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H28" s="38">
+      <c r="H28" s="35">
         <v>510</v>
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="42">
+      <c r="D29" s="39">
         <v>19.999999999999464</v>
       </c>
-      <c r="E29" s="42">
-        <v>0</v>
-      </c>
-      <c r="F29" s="38">
+      <c r="E29" s="39">
+        <v>0</v>
+      </c>
+      <c r="F29" s="35">
         <v>655</v>
       </c>
-      <c r="G29" s="38">
+      <c r="G29" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="35">
         <v>635.00000000000057</v>
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="38" t="s">
+      <c r="C30" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="42">
+      <c r="D30" s="39">
         <v>100.00000000000065</v>
       </c>
-      <c r="E30" s="42">
-        <v>0</v>
-      </c>
-      <c r="F30" s="38">
+      <c r="E30" s="39">
+        <v>0</v>
+      </c>
+      <c r="F30" s="35">
         <v>575</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G30" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="35">
         <v>474.99999999999937</v>
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="42">
+      <c r="D31" s="39">
         <v>8.7707618945387341E-14</v>
       </c>
-      <c r="E31" s="42">
-        <v>0</v>
-      </c>
-      <c r="F31" s="38">
+      <c r="E31" s="39">
+        <v>0</v>
+      </c>
+      <c r="F31" s="35">
         <v>680</v>
       </c>
-      <c r="G31" s="38">
+      <c r="G31" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H31" s="38">
+      <c r="H31" s="35">
         <v>679.99999999999989</v>
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="42">
+      <c r="D32" s="39">
         <v>450</v>
       </c>
-      <c r="E32" s="42">
+      <c r="E32" s="39">
         <v>-1000.0000000000382</v>
       </c>
-      <c r="F32" s="38">
+      <c r="F32" s="35">
         <v>450</v>
       </c>
-      <c r="G32" s="38">
+      <c r="G32" s="35">
         <v>12.500000000000059</v>
       </c>
-      <c r="H32" s="38">
+      <c r="H32" s="35">
         <v>2.4999999999999285</v>
       </c>
     </row>
     <row r="33" spans="2:8">
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="42">
+      <c r="D33" s="39">
         <v>2.2204460492502539E-15</v>
       </c>
-      <c r="E33" s="42">
-        <v>0</v>
-      </c>
-      <c r="F33" s="38">
+      <c r="E33" s="39">
+        <v>0</v>
+      </c>
+      <c r="F33" s="35">
         <v>490</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="35">
         <v>1E+30</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="35">
         <v>490.00000000000011</v>
       </c>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="42">
+      <c r="D34" s="39">
         <v>55.000000000000099</v>
       </c>
-      <c r="E34" s="42">
-        <v>0</v>
-      </c>
-      <c r="F34" s="38">
-        <v>0</v>
-      </c>
-      <c r="G34" s="38">
+      <c r="E34" s="39">
+        <v>0</v>
+      </c>
+      <c r="F34" s="35">
+        <v>0</v>
+      </c>
+      <c r="G34" s="35">
         <v>55.000000000000099</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="35">
         <v>1E+30</v>
       </c>
     </row>
     <row r="35" spans="2:8">
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="39">
         <v>600</v>
       </c>
-      <c r="E35" s="42">
-        <v>0</v>
-      </c>
-      <c r="F35" s="38">
-        <v>0</v>
-      </c>
-      <c r="G35" s="38">
+      <c r="E35" s="39">
+        <v>0</v>
+      </c>
+      <c r="F35" s="35">
+        <v>0</v>
+      </c>
+      <c r="G35" s="35">
         <v>600</v>
       </c>
-      <c r="H35" s="38">
+      <c r="H35" s="35">
         <v>1E+30</v>
       </c>
     </row>
     <row r="36" spans="2:8">
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="42">
-        <v>0</v>
-      </c>
-      <c r="E36" s="42">
+      <c r="D36" s="39">
+        <v>0</v>
+      </c>
+      <c r="E36" s="39">
         <v>2499.9999999999773</v>
       </c>
-      <c r="F36" s="38">
-        <v>0</v>
-      </c>
-      <c r="G36" s="38">
+      <c r="F36" s="35">
+        <v>0</v>
+      </c>
+      <c r="G36" s="35">
         <v>33.333333333333471</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:8">
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="42">
+      <c r="D37" s="39">
         <v>19.999999999999464</v>
       </c>
-      <c r="E37" s="42">
-        <v>0</v>
-      </c>
-      <c r="F37" s="38">
-        <v>0</v>
-      </c>
-      <c r="G37" s="38">
+      <c r="E37" s="39">
+        <v>0</v>
+      </c>
+      <c r="F37" s="35">
+        <v>0</v>
+      </c>
+      <c r="G37" s="35">
         <v>19.999999999999467</v>
       </c>
-      <c r="H37" s="38">
+      <c r="H37" s="35">
         <v>1E+30</v>
       </c>
     </row>
     <row r="38" spans="2:8">
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="42">
+      <c r="D38" s="39">
         <v>100.00000000000065</v>
       </c>
-      <c r="E38" s="42">
-        <v>0</v>
-      </c>
-      <c r="F38" s="38">
-        <v>0</v>
-      </c>
-      <c r="G38" s="38">
+      <c r="E38" s="39">
+        <v>0</v>
+      </c>
+      <c r="F38" s="35">
+        <v>0</v>
+      </c>
+      <c r="G38" s="35">
         <v>100.00000000000065</v>
       </c>
-      <c r="H38" s="38">
+      <c r="H38" s="35">
         <v>1E+30</v>
       </c>
     </row>
     <row r="39" spans="2:8">
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="C39" s="38" t="s">
+      <c r="C39" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="42">
+      <c r="D39" s="39">
         <v>8.7707618945387341E-14</v>
       </c>
-      <c r="E39" s="42">
+      <c r="E39" s="39">
         <v>1500.0000000000166</v>
       </c>
-      <c r="F39" s="38">
-        <v>0</v>
-      </c>
-      <c r="G39" s="38">
+      <c r="F39" s="35">
+        <v>0</v>
+      </c>
+      <c r="G39" s="35">
         <v>50.000000000000348</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:8">
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="42">
+      <c r="D40" s="39">
         <v>450</v>
       </c>
-      <c r="E40" s="42">
-        <v>0</v>
-      </c>
-      <c r="F40" s="38">
-        <v>0</v>
-      </c>
-      <c r="G40" s="38">
+      <c r="E40" s="39">
+        <v>0</v>
+      </c>
+      <c r="F40" s="35">
+        <v>0</v>
+      </c>
+      <c r="G40" s="35">
         <v>450</v>
       </c>
-      <c r="H40" s="38">
+      <c r="H40" s="35">
         <v>1E+30</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="16.5" thickBot="1">
-      <c r="B41" s="39" t="s">
+      <c r="B41" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="43">
+      <c r="D41" s="40">
         <v>2.2204460492502539E-15</v>
       </c>
-      <c r="E41" s="43">
+      <c r="E41" s="40">
         <v>499.99999999998431</v>
       </c>
-      <c r="F41" s="39">
-        <v>0</v>
-      </c>
-      <c r="G41" s="39">
+      <c r="F41" s="36">
+        <v>0</v>
+      </c>
+      <c r="G41" s="36">
         <v>10.00000000000005</v>
       </c>
-      <c r="H41" s="39">
+      <c r="H41" s="36">
         <v>0</v>
       </c>
     </row>
@@ -2144,6 +2163,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="87.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K44"/>
   <sheetViews>
@@ -2343,10 +2448,10 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B8" s="45"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="24" t="s">
@@ -2390,16 +2495,16 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="2"/>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="34"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="45"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="7"/>
@@ -2458,10 +2563,10 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="34"/>
+      <c r="B19" s="45"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="28" t="s">
@@ -2474,10 +2579,10 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2"/>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="45"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="6"/>
@@ -2766,63 +2871,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="87.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>